<commit_message>
delete akm fire selector
</commit_message>
<xml_diff>
--- a/changes/ak-parts.xlsx
+++ b/changes/ak-parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F13752-131E-4B32-B4CB-5F9656D1C2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756892FE-AD31-4F42-9ABA-E91FB39DF928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="182">
   <si>
     <t>new</t>
   </si>
@@ -261,12 +261,6 @@
   </si>
   <si>
     <t>Izhmash AK-74 Fire Selector</t>
-  </si>
-  <si>
-    <t>izhmash_akm_fire_selector</t>
-  </si>
-  <si>
-    <t>Izhmash AKM Fire Selector</t>
   </si>
   <si>
     <t>retro_arms_cnc_ak_model_a_fire_selector</t>
@@ -1433,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R94"/>
+  <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,7 +1517,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N64" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
+        <f t="shared" ref="N4:N63" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
         <v>-6.6000000000000005</v>
       </c>
     </row>
@@ -1842,7 +1836,7 @@
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1862,10 +1856,10 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
@@ -1891,10 +1885,10 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
@@ -1920,10 +1914,10 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
@@ -1949,10 +1943,10 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
@@ -2301,10 +2295,10 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C35" s="1">
         <v>6</v>
@@ -2334,10 +2328,10 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C36" s="1">
         <v>3</v>
@@ -2388,10 +2382,10 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C38" s="1">
         <v>0</v>
@@ -2417,10 +2411,10 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C39" s="1">
         <v>0</v>
@@ -2446,16 +2440,16 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" s="1">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2466,11 +2460,11 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="N40">
         <f t="shared" si="0"/>
-        <v>-0.4</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -2481,10 +2475,10 @@
         <v>79</v>
       </c>
       <c r="C41" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D41" s="1">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2495,26 +2489,20 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1">
-        <v>750</v>
+        <v>900</v>
       </c>
       <c r="N41">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="D42" s="1">
-        <v>0.03</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -2523,21 +2511,25 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="1">
-        <v>900</v>
-      </c>
+      <c r="M42" s="1"/>
       <c r="N42">
         <f t="shared" si="0"/>
-        <v>0.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="B43" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.03</v>
+      </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -2546,10 +2538,12 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
+      <c r="M43" s="1">
+        <v>300</v>
+      </c>
       <c r="N43">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -2563,7 +2557,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="1">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2578,7 +2572,7 @@
       </c>
       <c r="N44">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -2586,13 +2580,13 @@
         <v>86</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C45" s="1">
         <v>1</v>
       </c>
       <c r="D45" s="1">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2607,22 +2601,16 @@
       </c>
       <c r="N45">
         <f t="shared" si="0"/>
-        <v>0.19999999999999996</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>88</v>
-      </c>
+      <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="1">
-        <v>1</v>
-      </c>
-      <c r="D46" s="1">
-        <v>0.02</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -2631,21 +2619,25 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
-      <c r="M46" s="1">
-        <v>300</v>
-      </c>
+      <c r="M46" s="1"/>
       <c r="N46">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="B47" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="C47" s="1">
+        <v>2</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.03</v>
+      </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -2654,10 +2646,12 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
+      <c r="M47" s="1">
+        <v>750</v>
+      </c>
       <c r="N47">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -2668,10 +2662,10 @@
         <v>106</v>
       </c>
       <c r="C48" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D48" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2682,26 +2676,20 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1">
-        <v>750</v>
+        <v>600</v>
       </c>
       <c r="N48">
         <f t="shared" si="0"/>
-        <v>1.4</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C49" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="D49" s="1">
-        <v>0.02</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2710,21 +2698,25 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
-      <c r="M49" s="1">
-        <v>600</v>
-      </c>
+      <c r="M49" s="1"/>
       <c r="N49">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
+      <c r="A50" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="B50" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.02</v>
+      </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -2733,18 +2725,20 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
+      <c r="M50" s="1">
+        <v>0</v>
+      </c>
       <c r="N50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C51" s="1">
         <v>0</v>
@@ -2770,10 +2764,10 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C52" s="1">
         <v>0</v>
@@ -2798,18 +2792,12 @@
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" s="1">
-        <v>0</v>
-      </c>
-      <c r="D53" s="1">
-        <v>0.02</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -2818,21 +2806,25 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
-      <c r="M53" s="1">
-        <v>0</v>
-      </c>
+      <c r="M53" s="1"/>
       <c r="N53">
         <f t="shared" si="0"/>
-        <v>-0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="B54" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.04</v>
+      </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -2841,18 +2833,20 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
+      <c r="M54" s="1">
+        <v>0</v>
+      </c>
       <c r="N54">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C55" s="1">
         <v>0</v>
@@ -2878,10 +2872,10 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C56" s="1">
         <v>0</v>
@@ -2906,18 +2900,12 @@
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C57" s="1">
-        <v>0</v>
-      </c>
-      <c r="D57" s="1">
-        <v>0.04</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -2926,21 +2914,25 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
-      <c r="M57" s="1">
-        <v>0</v>
-      </c>
+      <c r="M57" s="1"/>
       <c r="N57">
-        <f t="shared" si="0"/>
-        <v>-0.8</v>
+        <f>C57-D57*20-E57*0.8-F57*0.6-H57*5+I57*10+J57/300</f>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="B58" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
+        <v>110</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0.23</v>
+      </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -2949,24 +2941,26 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
+      <c r="M58" s="1">
+        <v>0</v>
+      </c>
       <c r="N58">
         <f>C58-D58*20-E58*0.8-F58*0.6-H58*5+I58*10+J58/300</f>
-        <v>0</v>
+        <v>-4.6000000000000005</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C59" s="1">
         <v>0</v>
       </c>
       <c r="D59" s="1">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -2981,15 +2975,15 @@
       </c>
       <c r="N59">
         <f>C59-D59*20-E59*0.8-F59*0.6-H59*5+I59*10+J59/300</f>
-        <v>-4.6000000000000005</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C60" s="1">
         <v>0</v>
@@ -3024,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="D61" s="1">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -3039,22 +3033,19 @@
       </c>
       <c r="N61">
         <f>C61-D61*20-E61*0.8-F61*0.6-H61*5+I61*10+J61/300</f>
-        <v>-4</v>
+        <v>-4.2</v>
+      </c>
+      <c r="R61" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>115</v>
-      </c>
+      <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C62" s="1">
-        <v>0</v>
-      </c>
-      <c r="D62" s="1">
-        <v>0.21</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -3063,24 +3054,25 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
-      <c r="M62" s="1">
-        <v>0</v>
-      </c>
+      <c r="M62" s="1"/>
       <c r="N62">
-        <f>C62-D62*20-E62*0.8-F62*0.6-H62*5+I62*10+J62/300</f>
-        <v>-4.2</v>
-      </c>
-      <c r="R62" t="s">
-        <v>125</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
+      <c r="A63" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="B63" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
+        <v>129</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0.05</v>
+      </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -3089,18 +3081,20 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
+      <c r="M63" s="1">
+        <v>0</v>
+      </c>
       <c r="N63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C64" s="1">
         <v>0</v>
@@ -3120,22 +3114,22 @@
         <v>0</v>
       </c>
       <c r="N64">
-        <f t="shared" si="0"/>
+        <f>C64-D64*20-E64*0.8-F64*0.6-H64*5+I64*10+J64/300</f>
         <v>-1</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C65" s="1">
         <v>0</v>
       </c>
       <c r="D65" s="1">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -3150,7 +3144,7 @@
       </c>
       <c r="N65">
         <f>C65-D65*20-E65*0.8-F65*0.6-H65*5+I65*10+J65/300</f>
-        <v>-1</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
@@ -3178,23 +3172,17 @@
         <v>0</v>
       </c>
       <c r="N66">
-        <f>C66-D66*20-E66*0.8-F66*0.6-H66*5+I66*10+J66/300</f>
+        <f t="shared" ref="N66:N67" si="2">C66-D66*20-E66*0.8-F66*0.6-H66*5+I66*10+J66/300</f>
         <v>-0.4</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C67" s="1">
-        <v>0</v>
-      </c>
-      <c r="D67" s="1">
-        <v>0.02</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -3203,21 +3191,25 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
-      <c r="M67" s="1">
-        <v>0</v>
-      </c>
+      <c r="M67" s="1"/>
       <c r="N67">
-        <f t="shared" ref="N67:N68" si="2">C67-D67*20-E67*0.8-F67*0.6-H67*5+I67*10+J67/300</f>
-        <v>-0.4</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
+      <c r="A68" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="B68" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
+        <v>139</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0.1</v>
+      </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -3226,18 +3218,20 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
+      <c r="M68" s="1">
+        <v>0</v>
+      </c>
       <c r="N68">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="N68:N93" si="3">C68-D68*20-E68*0.8-F68*0.6-H68*5+I68*10+J68/300</f>
+        <v>-2</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C69" s="1">
         <v>0</v>
@@ -3257,7 +3251,7 @@
         <v>0</v>
       </c>
       <c r="N69">
-        <f t="shared" ref="N69:N94" si="3">C69-D69*20-E69*0.8-F69*0.6-H69*5+I69*10+J69/300</f>
+        <f t="shared" si="3"/>
         <v>-2</v>
       </c>
     </row>
@@ -3269,10 +3263,10 @@
         <v>137</v>
       </c>
       <c r="C70" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" s="1">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -3283,19 +3277,19 @@
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N70">
         <f t="shared" si="3"/>
-        <v>-2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C71" s="1">
         <v>1</v>
@@ -3312,7 +3306,7 @@
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="N71">
         <f t="shared" si="3"/>
@@ -3327,10 +3321,10 @@
         <v>148</v>
       </c>
       <c r="C72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72" s="1">
-        <v>0.13</v>
+        <v>0.06</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -3345,22 +3339,16 @@
       </c>
       <c r="N72">
         <f t="shared" si="3"/>
-        <v>-1.6</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>149</v>
-      </c>
+      <c r="A73" s="1"/>
       <c r="B73" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C73" s="1">
-        <v>0</v>
-      </c>
-      <c r="D73" s="1">
-        <v>0.06</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -3369,21 +3357,25 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
-      <c r="M73" s="1">
-        <v>0</v>
-      </c>
+      <c r="M73" s="1"/>
       <c r="N73">
         <f t="shared" si="3"/>
-        <v>-1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
+      <c r="A74" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B74" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0.1</v>
+      </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -3392,24 +3384,26 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
+      <c r="M74" s="1">
+        <v>0</v>
+      </c>
       <c r="N74">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C75" s="1">
         <v>0</v>
       </c>
       <c r="D75" s="1">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -3424,36 +3418,25 @@
       </c>
       <c r="N75">
         <f t="shared" si="3"/>
-        <v>-2</v>
+        <v>-1.7999999999999998</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C76" s="1">
-        <v>0</v>
-      </c>
-      <c r="D76" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="L76" s="1"/>
+      <c r="A76" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" t="s">
+        <v>150</v>
+      </c>
+      <c r="D76">
+        <v>0.05</v>
+      </c>
       <c r="M76" s="1">
         <v>0</v>
       </c>
       <c r="N76">
         <f t="shared" si="3"/>
-        <v>-1.7999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
@@ -3463,53 +3446,56 @@
       <c r="B77" t="s">
         <v>152</v>
       </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
       <c r="D77">
-        <v>0.05</v>
-      </c>
-      <c r="M77" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="M77">
         <v>0</v>
       </c>
       <c r="N77">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="B78" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B78" t="s">
-        <v>154</v>
-      </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-      <c r="D78">
-        <v>0.1</v>
-      </c>
-      <c r="M78">
-        <v>0</v>
       </c>
       <c r="N78">
         <f t="shared" si="3"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B79" s="1" t="s">
+      <c r="A79" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" t="s">
         <v>155</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0.08</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
       </c>
       <c r="N79">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B80" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -3536,14 +3522,14 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="M81">
         <v>0</v>
       </c>
       <c r="N81">
         <f t="shared" si="3"/>
-        <v>-1.6</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
@@ -3569,67 +3555,67 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B83" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83">
-        <v>0.05</v>
+        <v>0.12</v>
+      </c>
+      <c r="E83">
+        <v>-1</v>
+      </c>
+      <c r="F83">
+        <v>-1</v>
       </c>
       <c r="M83">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N83">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>-0.99999999999999989</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>158</v>
-      </c>
       <c r="B84" t="s">
-        <v>159</v>
-      </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-      <c r="D84">
-        <v>0.12</v>
-      </c>
-      <c r="E84">
-        <v>-1</v>
-      </c>
-      <c r="F84">
-        <v>-1</v>
-      </c>
-      <c r="M84">
-        <v>800</v>
+        <v>164</v>
       </c>
       <c r="N84">
         <f t="shared" si="3"/>
-        <v>-0.99999999999999989</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>169</v>
+      </c>
       <c r="B85" t="s">
-        <v>166</v>
+        <v>170</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0.06</v>
+      </c>
+      <c r="M85">
+        <v>0</v>
       </c>
       <c r="N85">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B86" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -3653,68 +3639,68 @@
         <v>168</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D87">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="M87">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="N87">
         <f t="shared" si="3"/>
-        <v>-1.2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>169</v>
-      </c>
       <c r="B88" t="s">
-        <v>170</v>
-      </c>
-      <c r="C88">
-        <v>1</v>
-      </c>
-      <c r="D88">
-        <v>0.1</v>
-      </c>
-      <c r="M88">
-        <v>500</v>
+        <v>171</v>
       </c>
       <c r="N88">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>176</v>
+      </c>
       <c r="B89" t="s">
-        <v>173</v>
+        <v>177</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0.04</v>
+      </c>
+      <c r="M89">
+        <v>0</v>
       </c>
       <c r="N89">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B90" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C90">
         <v>0</v>
       </c>
       <c r="D90">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="M90">
         <v>0</v>
       </c>
       <c r="N90">
         <f t="shared" si="3"/>
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -3725,38 +3711,38 @@
         <v>175</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D91">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="M91">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="N91">
         <f t="shared" si="3"/>
-        <v>-1.2</v>
+        <v>-0.40000000000000013</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B92" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D92">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="M92">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="N92">
         <f t="shared" si="3"/>
-        <v>-0.40000000000000013</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -3770,33 +3756,12 @@
         <v>0</v>
       </c>
       <c r="D93">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="M93">
         <v>0</v>
       </c>
       <c r="N93">
-        <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>182</v>
-      </c>
-      <c r="B94" t="s">
-        <v>183</v>
-      </c>
-      <c r="C94">
-        <v>0</v>
-      </c>
-      <c r="D94">
-        <v>0.04</v>
-      </c>
-      <c r="M94">
-        <v>0</v>
-      </c>
-      <c r="N94">
         <f t="shared" si="3"/>
         <v>-0.8</v>
       </c>

</xml_diff>

<commit_message>
increase weight and recoil of aks74u slightly
</commit_message>
<xml_diff>
--- a/changes/ak-parts.xlsx
+++ b/changes/ak-parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54BB33F3-F0D8-44DE-88CE-D49FDAB94235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A04E646-60AA-456C-836D-CAF827363B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1429,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,14 +1553,14 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="M6">
         <v>5000</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>-5.2</v>
+        <v>-5.4</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1574,14 +1574,20 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0.3</v>
+        <v>0.32</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-8.1999999999999993</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1990,7 +1996,7 @@
         <v>6</v>
       </c>
       <c r="D27" s="1">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E27" s="1">
         <v>-3</v>
@@ -2009,7 +2015,7 @@
       </c>
       <c r="N27">
         <f t="shared" si="0"/>
-        <v>8.6000000000000014</v>
+        <v>8.4</v>
       </c>
       <c r="P27">
         <v>3.2</v>
@@ -2030,7 +2036,7 @@
         <v>7</v>
       </c>
       <c r="D28" s="1">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E28" s="1">
         <v>-3</v>
@@ -2049,7 +2055,7 @@
       </c>
       <c r="N28">
         <f t="shared" si="0"/>
-        <v>9.8000000000000007</v>
+        <v>9.6</v>
       </c>
       <c r="Q28">
         <f t="shared" si="1"/>
@@ -2067,7 +2073,7 @@
         <v>8</v>
       </c>
       <c r="D29" s="1">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="E29" s="1">
         <v>-2</v>
@@ -2086,7 +2092,7 @@
       </c>
       <c r="N29">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="Q29">
         <f t="shared" si="1"/>
@@ -2104,7 +2110,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="1">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="E30" s="1">
         <v>-2</v>
@@ -2123,7 +2129,7 @@
       </c>
       <c r="N30">
         <f t="shared" si="0"/>
-        <v>2.8</v>
+        <v>2.5999999999999996</v>
       </c>
       <c r="P30">
         <v>6.8</v>
@@ -2144,7 +2150,7 @@
         <v>3</v>
       </c>
       <c r="D31" s="1">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="E31" s="1">
         <v>-3</v>
@@ -2163,7 +2169,7 @@
       </c>
       <c r="N31">
         <f t="shared" si="0"/>
-        <v>3.0000000000000009</v>
+        <v>2.8000000000000007</v>
       </c>
       <c r="P31">
         <v>7.5839100000000004</v>
@@ -2184,7 +2190,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="1">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="E32" s="1">
         <v>-4</v>
@@ -2203,7 +2209,7 @@
       </c>
       <c r="N32">
         <f t="shared" si="0"/>
-        <v>2.6</v>
+        <v>2.4</v>
       </c>
       <c r="P32">
         <v>8.1130200000000006</v>
@@ -2224,7 +2230,7 @@
         <v>4</v>
       </c>
       <c r="D33" s="1">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="E33" s="1">
         <v>-4</v>
@@ -2243,7 +2249,7 @@
       </c>
       <c r="N33">
         <f t="shared" si="0"/>
-        <v>3.8</v>
+        <v>3.6000000000000005</v>
       </c>
       <c r="P33">
         <v>9.6999999999999993</v>
@@ -2264,7 +2270,7 @@
         <v>5</v>
       </c>
       <c r="D34" s="1">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="E34" s="1">
         <v>-1</v>
@@ -2283,7 +2289,7 @@
       </c>
       <c r="N34">
         <f t="shared" si="0"/>
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="P34">
         <v>5.9965799999999998</v>
@@ -2304,7 +2310,7 @@
         <v>6</v>
       </c>
       <c r="D35" s="1">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E35" s="1">
         <v>-3</v>
@@ -2323,7 +2329,7 @@
       </c>
       <c r="N35">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -2337,7 +2343,7 @@
         <v>3</v>
       </c>
       <c r="D36" s="1">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="E36" s="1">
         <v>-2</v>
@@ -2356,7 +2362,7 @@
       </c>
       <c r="N36">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>